<commit_message>
update template of supplier bundles
</commit_message>
<xml_diff>
--- a/docs/.vuepress/public/supplier_bundles_tpl.xlsx
+++ b/docs/.vuepress/public/supplier_bundles_tpl.xlsx
@@ -65,7 +65,30 @@
     <t>Publisher domain</t>
   </si>
   <si>
-    <t>Relationship</t>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Relationship(*</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color rgb="FFFF0000"/>
+      </rPr>
+      <t>required</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>)</t>
+    </r>
   </si>
   <si>
     <r>
@@ -530,7 +553,7 @@
     <col customWidth="1" min="4" max="4" width="18.14"/>
     <col customWidth="1" min="5" max="5" width="20.57"/>
     <col customWidth="1" min="6" max="6" width="19.14"/>
-    <col customWidth="1" min="7" max="7" width="15.29"/>
+    <col customWidth="1" min="7" max="7" width="30.14"/>
     <col customWidth="1" min="8" max="8" width="20.86"/>
     <col customWidth="1" min="10" max="10" width="26.0"/>
     <col customWidth="1" min="11" max="11" width="59.14"/>

</xml_diff>